<commit_message>
plotting in silico go term heatmap uncondensed
</commit_message>
<xml_diff>
--- a/analyses/unipept/GO-terms/CC-GO-summary-insilico.xlsx
+++ b/analyses/unipept/GO-terms/CC-GO-summary-insilico.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="322" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="330" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="331" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="332" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="GO totals" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="187">
   <si>
     <t xml:space="preserve">Peptides</t>
   </si>
@@ -68,52 +69,184 @@
     <t xml:space="preserve">cytosol</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0016020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0045261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proton-transporting ATP synthase complex, catalytic core F(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0022627</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cytosolic small ribosomal subunit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0015935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small ribosomal subunit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photosystem I reaction center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0030126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPI vesicle coat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0000139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golgi membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photosystem I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:1990904</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ribonucleoprotein complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0043231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intracellular membrane-bounded organelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nucleus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0000220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacuolar proton-transporting V-type ATPase, V0 domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golgi apparatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005793</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endoplasmic reticulum-Golgi intermediate compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005783</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endoplasmic reticulum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0031361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integral component of thylakoid membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photosystem II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005840</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ribosome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0016471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacuolar proton-transporting V-type ATPase complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plasma membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chloroplast envelope</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0005739</t>
   </si>
   <si>
     <t xml:space="preserve">mitochondrion</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0045261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proton-transporting ATP synthase complex, catalytic core F(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005840</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ribosome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005634</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nucleus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005623</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009941</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chloroplast envelope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0022627</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cytosolic small ribosomal subunit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0016020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">membrane</t>
+    <t xml:space="preserve">GO:0000145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exocyst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endoplasmic reticulum lumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0034663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endoplasmic reticulum chaperone complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0010494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cytoplasmic stress granule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0002189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ribose phosphate diphosphokinase complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0045263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proton-transporting ATP synthase complex, coupling factor F(o)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009536</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plastid</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0022625</t>
@@ -122,10 +255,88 @@
     <t xml:space="preserve">cytosolic large ribosomal subunit</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0009523</t>
-  </si>
-  <si>
-    <t xml:space="preserve">photosystem II</t>
+    <t xml:space="preserve">GO:0000275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mitochondrial proton-transporting ATP synthase complex, catalytic core F(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009579</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thylakoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mitochondrial inner membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0033179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proton-transporting V-type ATPase, V0 domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005856</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cytoskeleton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0000786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nucleosome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chloroplast thylakoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0000790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuclear chromatin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacuolar membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mitochondrial respiratory chain complex III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0030076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light-harvesting complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photosystem II reaction center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photosystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nucleolus</t>
   </si>
   <si>
     <t xml:space="preserve">GO:0034098</t>
@@ -134,132 +345,36 @@
     <t xml:space="preserve">VCP-NPL4-UFD1 AAA ATPase complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005886</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plasma membrane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009522</t>
-  </si>
-  <si>
-    <t xml:space="preserve">photosystem I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:1990904</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ribonucleoprotein complex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0043231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intracellular membrane-bounded organelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009538</t>
-  </si>
-  <si>
-    <t xml:space="preserve">photosystem I reaction center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0034663</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endoplasmic reticulum chaperone complex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0031361</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integral component of thylakoid membrane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005788</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endoplasmic reticulum lumen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0015935</t>
-  </si>
-  <si>
-    <t xml:space="preserve">small ribosomal subunit</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0015934</t>
   </si>
   <si>
     <t xml:space="preserve">large ribosomal subunit</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0033179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proton-transporting V-type ATPase, V0 domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005783</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endoplasmic reticulum</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0000015</t>
   </si>
   <si>
     <t xml:space="preserve">phosphopyruvate hydratase complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0045263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proton-transporting ATP synthase complex, coupling factor F(o)</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0005765</t>
   </si>
   <si>
     <t xml:space="preserve">lysosomal membrane</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0016471</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vacuolar proton-transporting V-type ATPase complex</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0009654</t>
   </si>
   <si>
     <t xml:space="preserve">photosystem II oxygen evolving complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0000275</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mitochondrial proton-transporting ATP synthase complex, catalytic core F(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009536</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plastid</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0031207</t>
   </si>
   <si>
     <t xml:space="preserve">Sec62/Sec63 complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0009579</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thylakoid</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0032991</t>
   </si>
   <si>
@@ -332,18 +447,6 @@
     <t xml:space="preserve">mitochondrial proton-transporting ATP synthase complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005856</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cytoskeleton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005743</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mitochondrial inner membrane</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0005967</t>
   </si>
   <si>
@@ -362,18 +465,6 @@
     <t xml:space="preserve">3-isopropylmalate dehydratase complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0000786</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nucleosome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0000790</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nuclear chromatin</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0000502</t>
   </si>
   <si>
@@ -410,24 +501,6 @@
     <t xml:space="preserve">endoplasmic reticulum membrane</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0030076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">light-harvesting complex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009539</t>
-  </si>
-  <si>
-    <t xml:space="preserve">photosystem II reaction center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009521</t>
-  </si>
-  <si>
-    <t xml:space="preserve">photosystem</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0005960</t>
   </si>
   <si>
@@ -458,12 +531,6 @@
     <t xml:space="preserve">proteasome activator complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005750</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mitochondrial respiratory chain complex III</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0030686</t>
   </si>
   <si>
@@ -482,36 +549,18 @@
     <t xml:space="preserve">t-UTP complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005794</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golgi apparatus</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0030870</t>
   </si>
   <si>
     <t xml:space="preserve">Mre11 complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005774</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vacuolar membrane</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0008076</t>
   </si>
   <si>
     <t xml:space="preserve">voltage-gated potassium channel complex</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0009534</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chloroplast thylakoid</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0005871</t>
   </si>
   <si>
@@ -530,52 +579,16 @@
     <t xml:space="preserve">chromatin</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0030126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPI vesicle coat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0000139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golgi membrane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0000220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vacuolar proton-transporting V-type ATPase, V0 domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005793</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endoplasmic reticulum-Golgi intermediate compartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0000145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exocyst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0010494</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cytoplasmic stress granule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0002189</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ribose phosphate diphosphokinase complex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nucleolus</t>
+    <t xml:space="preserve">TermID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(obsolete) cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mitochondrial proton-transporting ATP synthase complex, catalytic sector F(1)</t>
   </si>
 </sst>
 </file>
@@ -585,7 +598,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -605,6 +618,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -649,8 +668,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -663,6 +686,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666666"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -671,14 +754,581 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -696,8 +1346,8 @@
   </sheetPr>
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -778,10 +1428,10 @@
         <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,10 +1450,10 @@
         <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -811,10 +1461,10 @@
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,10 +1472,10 @@
         <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,10 +1483,10 @@
         <v>21</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,10 +1494,10 @@
         <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,10 +1505,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,10 +1516,10 @@
         <v>17</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,10 +1527,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -888,10 +1538,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,10 +1549,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,10 +1560,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,10 +1571,10 @@
         <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,10 +1582,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -943,10 +1593,10 @@
         <v>11</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,10 +1604,10 @@
         <v>11</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,10 +1615,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,10 +1626,10 @@
         <v>9</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -987,10 +1637,10 @@
         <v>9</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,10 +1648,10 @@
         <v>8</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,10 +1659,10 @@
         <v>8</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,10 +1670,10 @@
         <v>8</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,10 +1681,10 @@
         <v>7</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,10 +1692,10 @@
         <v>6</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,10 +1703,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,10 +1714,10 @@
         <v>6</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,10 +1725,10 @@
         <v>6</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,10 +1736,10 @@
         <v>5</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,10 +1758,10 @@
         <v>5</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,10 +1769,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,10 +1780,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,10 +1791,10 @@
         <v>4</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,10 +1802,10 @@
         <v>4</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,10 +1813,10 @@
         <v>4</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,10 +1824,10 @@
         <v>4</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,10 +1835,10 @@
         <v>4</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,10 +1846,10 @@
         <v>4</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1207,10 +1857,10 @@
         <v>4</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,10 +1868,10 @@
         <v>4</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,10 +1879,10 @@
         <v>4</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1240,10 +1890,10 @@
         <v>4</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1251,10 +1901,10 @@
         <v>3</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,10 +1912,10 @@
         <v>3</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,10 +1923,10 @@
         <v>3</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1284,10 +1934,10 @@
         <v>3</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1295,10 +1945,10 @@
         <v>3</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1306,10 +1956,10 @@
         <v>3</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1317,10 +1967,10 @@
         <v>2</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,10 +1978,10 @@
         <v>2</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1339,10 +1989,10 @@
         <v>2</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,10 +2000,10 @@
         <v>2</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,10 +2011,10 @@
         <v>2</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,10 +2022,10 @@
         <v>2</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,10 +2033,10 @@
         <v>1</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1394,10 +2044,10 @@
         <v>1</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,10 +2055,10 @@
         <v>1</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,10 +2066,10 @@
         <v>1</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,10 +2077,10 @@
         <v>1</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1438,10 +2088,10 @@
         <v>1</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,10 +2110,10 @@
         <v>1</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,10 +2121,10 @@
         <v>1</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,10 +2132,10 @@
         <v>1</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,10 +2143,10 @@
         <v>1</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,10 +2154,10 @@
         <v>1</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,10 +2165,10 @@
         <v>1</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,10 +2176,10 @@
         <v>1</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,10 +2187,10 @@
         <v>1</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>151</v>
+        <v>37</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,10 +2198,10 @@
         <v>1</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1572,8 +2222,8 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1632,10 +2282,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1643,10 +2293,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,10 +2304,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,10 +2315,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1687,10 +2337,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1698,10 +2348,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,10 +2370,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,10 +2381,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,10 +2392,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,10 +2403,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,10 +2414,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,10 +2425,10 @@
         <v>2</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1786,10 +2436,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,10 +2447,10 @@
         <v>2</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,10 +2458,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,10 +2469,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,10 +2480,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1841,10 +2491,10 @@
         <v>2</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,10 +2502,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,10 +2513,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,10 +2524,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +2549,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1958,10 +2608,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,10 +2619,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,10 +2630,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,10 +2641,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,10 +2652,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,10 +2674,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,10 +2696,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2057,10 +2707,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>159</v>
+        <v>87</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>160</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,10 +2718,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,10 +2729,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,10 +2740,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2114,8 +2764,8 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2185,10 +2835,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,10 +2846,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2207,10 +2857,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,10 +2868,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,10 +2879,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,10 +2890,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,10 +2901,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2262,10 +2912,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,10 +2923,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,10 +2934,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,10 +2956,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2317,10 +2967,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,10 +2978,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2339,10 +2989,10 @@
         <v>2</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,10 +3011,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2372,10 +3022,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,10 +3033,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2407,8 +3057,8 @@
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2500,10 +3150,10 @@
         <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,10 +3161,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,10 +3172,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2533,10 +3183,10 @@
         <v>16</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2544,10 +3194,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>167</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>168</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2555,10 +3205,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>169</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>170</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2566,10 +3216,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2577,10 +3227,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2588,10 +3238,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,10 +3249,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,10 +3260,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2621,10 +3271,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2632,10 +3282,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,10 +3293,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,10 +3304,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2665,10 +3315,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,10 +3326,10 @@
         <v>6</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,10 +3348,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,10 +3359,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,10 +3370,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,10 +3381,10 @@
         <v>3</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,10 +3392,10 @@
         <v>3</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,10 +3403,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,10 +3414,10 @@
         <v>3</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2775,10 +3425,10 @@
         <v>2</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,10 +3436,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,10 +3447,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,10 +3458,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2832,8 +3482,8 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2892,10 +3542,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2914,10 +3564,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,10 +3575,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2936,10 +3586,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,10 +3597,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2958,10 +3608,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2991,17 +3641,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,552 +3667,827 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>197</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>139</v>
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B90"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E78" activeCellId="0" sqref="E78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="B63" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B22" s="0" t="s">
+    </row>
+    <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="B84" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B34" s="0" t="s">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="B86" s="0" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>182</v>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>